<commit_message>
ajout dans le même fichier
</commit_message>
<xml_diff>
--- a/RenduExcel.xlsx
+++ b/RenduExcel.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehdi\OneDrive\Documents\QualiDev\SEBBAK-FOUCHER-BALDONI-mesures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08E8A54C-E046-4D67-B495-8F30999AAA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941E32FB-2129-483E-BC00-D4C5B8A3D747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="3" xr2:uid="{BF111D66-066C-44FC-9E62-880C9479279D}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="19200" windowHeight="11170" activeTab="4" xr2:uid="{BF111D66-066C-44FC-9E62-880C9479279D}"/>
   </bookViews>
   <sheets>
     <sheet name="Loc" sheetId="1" r:id="rId1"/>
     <sheet name="CC" sheetId="2" r:id="rId2"/>
     <sheet name="Feuille de comptage" sheetId="3" r:id="rId3"/>
     <sheet name="UFC" sheetId="4" r:id="rId4"/>
+    <sheet name="UFC score" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Fichier</t>
   </si>
@@ -147,6 +148,42 @@
   </si>
   <si>
     <t>API externe</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
+  </si>
+  <si>
+    <t>Poids simple</t>
+  </si>
+  <si>
+    <t>Poids moyen</t>
+  </si>
+  <si>
+    <t>Poids difficile</t>
+  </si>
+  <si>
+    <t>Score Simple</t>
+  </si>
+  <si>
+    <t>Score Moyen</t>
+  </si>
+  <si>
+    <t>Score difficile</t>
+  </si>
+  <si>
+    <t>Entrées ext</t>
+  </si>
+  <si>
+    <t>Sorties ext</t>
+  </si>
+  <si>
+    <t>Requetes ext</t>
+  </si>
+  <si>
+    <t>Fichiers int</t>
+  </si>
+  <si>
+    <t>Fichiers ext</t>
   </si>
 </sst>
 </file>
@@ -859,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A52282-07ED-42EB-A326-84230F3701EE}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D6" si="0">B3*C3</f>
         <v>9</v>
       </c>
     </row>
@@ -965,6 +1002,188 @@
       <c r="D8">
         <f>SUM(D2:D6)</f>
         <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9353429-691A-4518-8A42-29528C60CA66}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -973,6 +1192,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="00e47fa2-6af5-44d7-9dc7-05f6e053fd25" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD41C8BA181F59419EAB8A93DFE5D116" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="950de2398ed76651633d861d1585b41f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="00e47fa2-6af5-44d7-9dc7-05f6e053fd25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46b83f6a5a00534dc19ea90c544a87b4" ns3:_="">
     <xsd:import namespace="00e47fa2-6af5-44d7-9dc7-05f6e053fd25"/>
@@ -1160,24 +1396,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F123D3E-927A-4371-BF73-704DC3E1E573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00e47fa2-6af5-44d7-9dc7-05f6e053fd25"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="00e47fa2-6af5-44d7-9dc7-05f6e053fd25" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7F120-296C-4137-9573-7986C8B7A866}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7309450A-6C16-4F0D-80A6-1A36542A4A4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1193,28 +1436,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E7F120-296C-4137-9573-7986C8B7A866}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F123D3E-927A-4371-BF73-704DC3E1E573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00e47fa2-6af5-44d7-9dc7-05f6e053fd25"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>